<commit_message>
add: cracksql & st-raptor
</commit_message>
<xml_diff>
--- a/src/paper_list.xlsx
+++ b/src/paper_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yizhang/Desktop/Data Agents Survey/awesome-data-agents/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6269A70-D128-1947-A475-A7A2AF823B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700975CE-AC5C-6248-9D15-E7C4C34CBF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5980" yWindow="2300" windowWidth="29400" windowHeight="18360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="L1" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="488">
   <si>
     <r>
       <rPr>
@@ -2612,6 +2612,30 @@
   </si>
   <si>
     <t>NeurIPS</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>ST-Raptor</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>ST-Raptor: LLM-Powered Semi-Structured Table Question Answering</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2508.18190</t>
+  </si>
+  <si>
+    <t>SIGMOD</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cracking SQL Barriers: An LLM-based Dialect Translation System</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3725278</t>
+  </si>
+  <si>
+    <t>CrackSQL</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -2619,7 +2643,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -2734,8 +2758,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="58">
+  <fills count="59">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3020,6 +3052,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF6425D0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE1EAFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3507,7 +3545,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3759,6 +3797,24 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="66" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="58" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="58" borderId="66" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="58" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="56" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4084,10 +4140,10 @@
   <dimension ref="A1:G237"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="13"/>
@@ -4341,8 +4397,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="19" customHeight="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="27"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="86"/>
       <c r="C13" s="54" t="s">
         <v>164</v>
       </c>
@@ -6832,9 +6888,9 @@
     <hyperlink ref="E44" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
     <hyperlink ref="E3" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
     <hyperlink ref="E12" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="E13" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="E36" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="E43" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="E36" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="E43" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="E13" r:id="rId53" xr:uid="{11FCC11B-99E2-6B4C-A9D4-EECA298CBFF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6845,11 +6901,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K251"/>
+  <dimension ref="A1:K253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="13"/>
@@ -7007,8 +7063,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="19" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="27"/>
+      <c r="A8" s="84"/>
+      <c r="B8" s="86"/>
       <c r="C8" s="54" t="s">
         <v>291</v>
       </c>
@@ -7027,39 +7083,39 @@
     </row>
     <row r="9" spans="1:7" ht="19" customHeight="1">
       <c r="A9" s="3"/>
-      <c r="B9" s="27" t="s">
-        <v>166</v>
-      </c>
+      <c r="B9" s="27"/>
       <c r="C9" s="54" t="s">
-        <v>293</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>294</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>295</v>
-      </c>
-      <c r="G9" s="27">
-        <v>2024</v>
+        <v>487</v>
+      </c>
+      <c r="D9" s="87" t="s">
+        <v>485</v>
+      </c>
+      <c r="E9" s="88" t="s">
+        <v>486</v>
+      </c>
+      <c r="F9" s="89" t="s">
+        <v>140</v>
+      </c>
+      <c r="G9" s="89">
+        <v>2025</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="19" customHeight="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="27"/>
+      <c r="B10" s="27" t="s">
+        <v>166</v>
+      </c>
       <c r="C10" s="54" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>147</v>
+        <v>295</v>
       </c>
       <c r="G10" s="27">
         <v>2024</v>
@@ -7069,117 +7125,117 @@
       <c r="A11" s="3"/>
       <c r="B11" s="27"/>
       <c r="C11" s="54" t="s">
+        <v>296</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="G11" s="27">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="19" customHeight="1">
+      <c r="A12" s="3"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="54" t="s">
         <v>298</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D12" s="28" t="s">
         <v>299</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E12" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F12" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G12" s="27">
         <v>2025</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="19" customHeight="1">
-      <c r="A12" s="8" t="s">
+    <row r="13" spans="1:7" ht="19" customHeight="1">
+      <c r="A13" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B13" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="C13" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D13" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E13" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="F13" s="33" t="s">
         <v>137</v>
-      </c>
-      <c r="G12" s="16">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="19" customHeight="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="58" t="s">
-        <v>302</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F13" s="33" t="s">
-        <v>304</v>
       </c>
       <c r="G13" s="16">
         <v>2024</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14">
-      <c r="A14" s="8"/>
+    <row r="14" spans="1:7" ht="19" customHeight="1">
+      <c r="A14" s="3"/>
       <c r="B14" s="16"/>
-      <c r="C14" s="57" t="s">
-        <v>305</v>
-      </c>
-      <c r="D14" s="51" t="s">
-        <v>306</v>
-      </c>
-      <c r="E14" s="51" t="s">
-        <v>104</v>
-      </c>
-      <c r="F14" s="50" t="s">
-        <v>147</v>
+      <c r="C14" s="58" t="s">
+        <v>302</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>304</v>
       </c>
       <c r="G14" s="16">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14">
-      <c r="A15" s="3" t="s">
-        <v>144</v>
-      </c>
+      <c r="A15" s="8"/>
       <c r="B15" s="16"/>
       <c r="C15" s="57" t="s">
-        <v>307</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="F15" s="33" t="s">
-        <v>309</v>
+        <v>305</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>306</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="50" t="s">
+        <v>147</v>
       </c>
       <c r="G15" s="16">
         <v>2025</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="19" customHeight="1">
-      <c r="A16" s="3"/>
+    <row r="16" spans="1:7" ht="14">
+      <c r="A16" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="B16" s="16"/>
       <c r="C16" s="57" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G16" s="16">
         <v>2025</v>
@@ -7188,17 +7244,17 @@
     <row r="17" spans="1:11" ht="19" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="16"/>
-      <c r="C17" s="58" t="s">
-        <v>313</v>
+      <c r="C17" s="57" t="s">
+        <v>310</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G17" s="16">
         <v>2025</v>
@@ -7207,17 +7263,17 @@
     <row r="18" spans="1:11" ht="19" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="16"/>
-      <c r="C18" s="57" t="s">
-        <v>316</v>
+      <c r="C18" s="58" t="s">
+        <v>313</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>147</v>
+        <v>315</v>
       </c>
       <c r="G18" s="16">
         <v>2025</v>
@@ -7225,58 +7281,58 @@
     </row>
     <row r="19" spans="1:11" ht="19" customHeight="1">
       <c r="A19" s="3"/>
-      <c r="B19" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="C19" s="59" t="s">
-        <v>318</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>319</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="F19" s="35" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="G19" s="35">
-        <v>2024</v>
+      <c r="G19" s="16">
+        <v>2025</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="19" customHeight="1">
       <c r="A20" s="3"/>
-      <c r="B20" s="35"/>
+      <c r="B20" s="35" t="s">
+        <v>186</v>
+      </c>
       <c r="C20" s="59" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F20" s="35" t="s">
-        <v>322</v>
+        <v>147</v>
       </c>
       <c r="G20" s="35">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="19" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="35"/>
       <c r="C21" s="59" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G21" s="35">
         <v>2025</v>
@@ -7284,39 +7340,39 @@
     </row>
     <row r="22" spans="1:11" ht="19" customHeight="1">
       <c r="A22" s="3"/>
-      <c r="B22" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C22" s="60" t="s">
-        <v>326</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="48" t="s">
-        <v>147</v>
-      </c>
-      <c r="G22" s="1">
-        <v>2024</v>
+      <c r="B22" s="35"/>
+      <c r="C22" s="59" t="s">
+        <v>323</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>325</v>
+      </c>
+      <c r="G22" s="35">
+        <v>2025</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="19" customHeight="1">
       <c r="A23" s="3"/>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="C23" s="60" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F23" s="48" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="G23" s="1">
         <v>2024</v>
@@ -7325,43 +7381,39 @@
     <row r="24" spans="1:11" ht="19" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="61" t="s">
-        <v>330</v>
+      <c r="C24" s="60" t="s">
+        <v>328</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F24" s="48" t="s">
-        <v>191</v>
+        <v>137</v>
       </c>
       <c r="G24" s="1">
         <v>2024</v>
       </c>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
     </row>
     <row r="25" spans="1:11" ht="19" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="60" t="s">
-        <v>332</v>
+      <c r="C25" s="61" t="s">
+        <v>330</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F25" s="48" t="s">
-        <v>137</v>
+        <v>191</v>
       </c>
       <c r="G25" s="1">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="H25" s="49"/>
       <c r="I25" s="49"/>
@@ -7371,36 +7423,40 @@
     <row r="26" spans="1:11" ht="19" customHeight="1">
       <c r="A26" s="3"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="61" t="s">
-        <v>334</v>
+      <c r="C26" s="60" t="s">
+        <v>332</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F26" s="48" t="s">
-        <v>336</v>
+        <v>137</v>
       </c>
       <c r="G26" s="1">
         <v>2025</v>
       </c>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
     </row>
     <row r="27" spans="1:11" ht="19" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="60" t="s">
-        <v>337</v>
+      <c r="C27" s="61" t="s">
+        <v>334</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F27" s="48" t="s">
-        <v>137</v>
+        <v>336</v>
       </c>
       <c r="G27" s="1">
         <v>2025</v>
@@ -7410,13 +7466,13 @@
       <c r="A28" s="3"/>
       <c r="B28" s="1"/>
       <c r="C28" s="60" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F28" s="48" t="s">
         <v>137</v>
@@ -7426,61 +7482,61 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="19" customHeight="1">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="3"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="60" t="s">
+        <v>339</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="19" customHeight="1">
+      <c r="A30" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="C29" s="62" t="s">
+      <c r="C30" s="62" t="s">
         <v>341</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E30" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="F29" s="40" t="s">
+      <c r="F30" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G30" s="7">
         <v>2023</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="19" customHeight="1">
-      <c r="A30" s="8"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="62" t="s">
-        <v>343</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="G30" s="7">
-        <v>2024</v>
-      </c>
-    </row>
     <row r="31" spans="1:11" ht="19" customHeight="1">
-      <c r="A31" s="3"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="7"/>
       <c r="C31" s="62" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F31" s="40" t="s">
-        <v>218</v>
+        <v>147</v>
       </c>
       <c r="G31" s="7">
         <v>2024</v>
@@ -7489,17 +7545,17 @@
     <row r="32" spans="1:11" ht="19" customHeight="1">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
-      <c r="C32" s="63" t="s">
-        <v>347</v>
+      <c r="C32" s="62" t="s">
+        <v>345</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F32" s="40" t="s">
-        <v>147</v>
+        <v>218</v>
       </c>
       <c r="G32" s="7">
         <v>2024</v>
@@ -7508,134 +7564,134 @@
     <row r="33" spans="1:8" ht="19" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="73" t="s">
+      <c r="C33" s="63" t="s">
+        <v>347</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="G33" s="7">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="19" customHeight="1">
+      <c r="A34" s="84"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="73" t="s">
         <v>349</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E34" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="40" t="s">
+      <c r="F34" s="40" t="s">
         <v>277</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G34" s="7">
         <v>2025</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="19" customHeight="1">
-      <c r="A34" s="3"/>
-      <c r="B34" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="C34" s="65" t="s">
-        <v>351</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F34" s="36" t="s">
-        <v>325</v>
-      </c>
-      <c r="G34" s="10">
-        <v>2023</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="19" customHeight="1">
       <c r="A35" s="3"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="65" t="s">
-        <v>353</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>354</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F35" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="G35" s="10">
-        <v>2024</v>
+      <c r="B35" s="7"/>
+      <c r="C35" s="73" t="s">
+        <v>481</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="F35" s="40" t="s">
+        <v>484</v>
+      </c>
+      <c r="G35" s="7">
+        <v>2026</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="19" customHeight="1">
       <c r="A36" s="3"/>
-      <c r="B36" s="10"/>
+      <c r="B36" s="10" t="s">
+        <v>225</v>
+      </c>
       <c r="C36" s="65" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F36" s="36" t="s">
-        <v>218</v>
+        <v>325</v>
       </c>
       <c r="G36" s="10">
-        <v>2024</v>
-      </c>
-      <c r="H36" s="41"/>
+        <v>2023</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="19" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="10"/>
       <c r="C37" s="65" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F37" s="36" t="s">
-        <v>359</v>
+        <v>137</v>
       </c>
       <c r="G37" s="10">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="19" customHeight="1">
       <c r="A38" s="3"/>
       <c r="B38" s="10"/>
       <c r="C38" s="65" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="F38" s="36" t="s">
-        <v>140</v>
+        <v>218</v>
       </c>
       <c r="G38" s="10">
-        <v>2025</v>
-      </c>
+        <v>2024</v>
+      </c>
+      <c r="H38" s="41"/>
     </row>
     <row r="39" spans="1:8" ht="19" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="10"/>
-      <c r="C39" s="64" t="s">
-        <v>362</v>
+      <c r="C39" s="65" t="s">
+        <v>357</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="F39" s="36" t="s">
-        <v>137</v>
+        <v>359</v>
       </c>
       <c r="G39" s="10">
         <v>2025</v>
@@ -7645,16 +7701,16 @@
       <c r="A40" s="3"/>
       <c r="B40" s="10"/>
       <c r="C40" s="65" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="F40" s="36" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G40" s="10">
         <v>2025</v>
@@ -7662,155 +7718,155 @@
     </row>
     <row r="41" spans="1:8" ht="19" customHeight="1">
       <c r="A41" s="3"/>
-      <c r="B41" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="C41" s="74" t="s">
-        <v>366</v>
-      </c>
-      <c r="D41" s="38" t="s">
-        <v>367</v>
-      </c>
-      <c r="E41" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F41" s="39" t="s">
-        <v>277</v>
-      </c>
-      <c r="G41" s="11">
-        <v>2024</v>
+      <c r="B41" s="10"/>
+      <c r="C41" s="64" t="s">
+        <v>362</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="G41" s="10">
+        <v>2025</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="19" customHeight="1">
       <c r="A42" s="3"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="75" t="s">
-        <v>368</v>
-      </c>
-      <c r="D42" s="38" t="s">
-        <v>369</v>
-      </c>
-      <c r="E42" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="F42" s="39" t="s">
-        <v>194</v>
-      </c>
-      <c r="G42" s="11">
-        <v>2024</v>
+      <c r="B42" s="10"/>
+      <c r="C42" s="65" t="s">
+        <v>364</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="G42" s="10">
+        <v>2025</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="19" customHeight="1">
       <c r="A43" s="3"/>
-      <c r="B43" s="11"/>
+      <c r="B43" s="11" t="s">
+        <v>235</v>
+      </c>
       <c r="C43" s="74" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E43" s="38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F43" s="39" t="s">
         <v>277</v>
       </c>
       <c r="G43" s="11">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="19" customHeight="1">
       <c r="A44" s="3"/>
       <c r="B44" s="11"/>
       <c r="C44" s="75" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E44" s="38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F44" s="39" t="s">
-        <v>241</v>
+        <v>194</v>
       </c>
       <c r="G44" s="11">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="19" customHeight="1">
       <c r="A45" s="3"/>
-      <c r="B45" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="C45" s="58" t="s">
-        <v>374</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>375</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F45" s="33" t="s">
-        <v>480</v>
-      </c>
-      <c r="G45" s="16">
-        <v>2023</v>
+      <c r="B45" s="11"/>
+      <c r="C45" s="74" t="s">
+        <v>370</v>
+      </c>
+      <c r="D45" s="38" t="s">
+        <v>371</v>
+      </c>
+      <c r="E45" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F45" s="39" t="s">
+        <v>277</v>
+      </c>
+      <c r="G45" s="11">
+        <v>2025</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="19" customHeight="1">
       <c r="A46" s="3"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="58" t="s">
-        <v>376</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>377</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F46" s="33" t="s">
-        <v>359</v>
-      </c>
-      <c r="G46" s="16">
-        <v>2024</v>
+      <c r="B46" s="11"/>
+      <c r="C46" s="75" t="s">
+        <v>372</v>
+      </c>
+      <c r="D46" s="38" t="s">
+        <v>373</v>
+      </c>
+      <c r="E46" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="F46" s="39" t="s">
+        <v>241</v>
+      </c>
+      <c r="G46" s="11">
+        <v>2025</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="19" customHeight="1">
       <c r="A47" s="3"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="57" t="s">
-        <v>378</v>
+      <c r="B47" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="C47" s="58" t="s">
+        <v>374</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="F47" s="33" t="s">
-        <v>194</v>
+        <v>480</v>
       </c>
       <c r="G47" s="16">
-        <v>2024</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="19" customHeight="1">
       <c r="A48" s="3"/>
       <c r="B48" s="16"/>
       <c r="C48" s="58" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F48" s="33" t="s">
-        <v>218</v>
+        <v>359</v>
       </c>
       <c r="G48" s="16">
         <v>2024</v>
@@ -7819,14 +7875,14 @@
     <row r="49" spans="1:7" ht="19" customHeight="1">
       <c r="A49" s="3"/>
       <c r="B49" s="16"/>
-      <c r="C49" s="58" t="s">
-        <v>382</v>
+      <c r="C49" s="57" t="s">
+        <v>378</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F49" s="33" t="s">
         <v>194</v>
@@ -7839,56 +7895,56 @@
       <c r="A50" s="3"/>
       <c r="B50" s="16"/>
       <c r="C50" s="58" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F50" s="33" t="s">
-        <v>147</v>
+        <v>218</v>
       </c>
       <c r="G50" s="16">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="19" customHeight="1">
       <c r="A51" s="3"/>
       <c r="B51" s="16"/>
-      <c r="C51" s="57" t="s">
-        <v>386</v>
+      <c r="C51" s="58" t="s">
+        <v>382</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F51" s="33" t="s">
-        <v>147</v>
+        <v>194</v>
       </c>
       <c r="G51" s="16">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="19" customHeight="1">
       <c r="A52" s="3"/>
       <c r="B52" s="16"/>
-      <c r="C52" s="57" t="s">
-        <v>388</v>
+      <c r="C52" s="58" t="s">
+        <v>384</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F52" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="G52" s="33">
+        <v>147</v>
+      </c>
+      <c r="G52" s="16">
         <v>2025</v>
       </c>
     </row>
@@ -7896,75 +7952,75 @@
       <c r="A53" s="3"/>
       <c r="B53" s="16"/>
       <c r="C53" s="57" t="s">
+        <v>386</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>387</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F53" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="G53" s="16">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="19" customHeight="1">
+      <c r="A54" s="3"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="57" t="s">
+        <v>388</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>389</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F54" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="G54" s="33">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="19" customHeight="1">
+      <c r="A55" s="3"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="57" t="s">
         <v>390</v>
       </c>
-      <c r="D53" s="15" t="s">
+      <c r="D55" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="E55" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="F53" s="33" t="s">
+      <c r="F55" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="G53" s="33">
+      <c r="G55" s="33">
         <v>2025</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="19" customHeight="1">
-      <c r="A54" s="42"/>
-      <c r="B54" s="17" t="s">
+    <row r="56" spans="1:7" ht="19" customHeight="1">
+      <c r="A56" s="42"/>
+      <c r="B56" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="C54" s="68" t="s">
+      <c r="C56" s="68" t="s">
         <v>392</v>
       </c>
-      <c r="D54" s="18" t="s">
+      <c r="D56" s="18" t="s">
         <v>393</v>
       </c>
-      <c r="E54" s="24" t="s">
+      <c r="E56" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F54" s="21" t="s">
+      <c r="F56" s="21" t="s">
         <v>194</v>
-      </c>
-      <c r="G54" s="43">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="19" customHeight="1">
-      <c r="A55" s="42"/>
-      <c r="B55" s="43"/>
-      <c r="C55" s="76" t="s">
-        <v>394</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>395</v>
-      </c>
-      <c r="E55" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F55" s="25" t="s">
-        <v>396</v>
-      </c>
-      <c r="G55" s="43">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="14">
-      <c r="A56" s="42"/>
-      <c r="B56" s="43"/>
-      <c r="C56" s="76" t="s">
-        <v>397</v>
-      </c>
-      <c r="D56" s="18" t="s">
-        <v>398</v>
-      </c>
-      <c r="E56" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="F56" s="25" t="s">
-        <v>266</v>
       </c>
       <c r="G56" s="43">
         <v>2024</v>
@@ -7973,74 +8029,74 @@
     <row r="57" spans="1:7" ht="19" customHeight="1">
       <c r="A57" s="42"/>
       <c r="B57" s="43"/>
-      <c r="C57" s="68" t="s">
-        <v>399</v>
+      <c r="C57" s="76" t="s">
+        <v>394</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="E57" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F57" s="25" t="s">
-        <v>137</v>
+        <v>396</v>
       </c>
       <c r="G57" s="43">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="19" customHeight="1">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="14">
       <c r="A58" s="42"/>
       <c r="B58" s="43"/>
-      <c r="C58" s="68" t="s">
-        <v>401</v>
+      <c r="C58" s="76" t="s">
+        <v>397</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E58" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F58" s="25" t="s">
-        <v>137</v>
+        <v>266</v>
       </c>
       <c r="G58" s="43">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="14">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="19" customHeight="1">
       <c r="A59" s="42"/>
       <c r="B59" s="43"/>
-      <c r="C59" s="76" t="s">
-        <v>403</v>
+      <c r="C59" s="68" t="s">
+        <v>399</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="E59" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F59" s="25" t="s">
-        <v>266</v>
+        <v>137</v>
       </c>
       <c r="G59" s="43">
         <v>2025</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="14">
+    <row r="60" spans="1:7" ht="19" customHeight="1">
       <c r="A60" s="42"/>
       <c r="B60" s="43"/>
-      <c r="C60" s="76" t="s">
-        <v>405</v>
+      <c r="C60" s="68" t="s">
+        <v>401</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="E60" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F60" s="25" t="s">
-        <v>241</v>
+        <v>137</v>
       </c>
       <c r="G60" s="43">
         <v>2025</v>
@@ -8050,13 +8106,13 @@
       <c r="A61" s="42"/>
       <c r="B61" s="43"/>
       <c r="C61" s="76" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E61" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F61" s="25" t="s">
         <v>266</v>
@@ -8069,13 +8125,13 @@
       <c r="A62" s="42"/>
       <c r="B62" s="43"/>
       <c r="C62" s="76" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E62" s="24" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="F62" s="25" t="s">
         <v>241</v>
@@ -8084,32 +8140,52 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="17">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="72"/>
-      <c r="D63" s="44"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="37"/>
-      <c r="G63" s="4"/>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="72"/>
-      <c r="D64" s="46"/>
-      <c r="E64" s="46"/>
-      <c r="F64" s="45"/>
-      <c r="G64" s="47"/>
-    </row>
-    <row r="65" spans="1:7">
+    <row r="63" spans="1:7" ht="14">
+      <c r="A63" s="42"/>
+      <c r="B63" s="43"/>
+      <c r="C63" s="76" t="s">
+        <v>407</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="E63" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="F63" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="G63" s="43">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="14">
+      <c r="A64" s="42"/>
+      <c r="B64" s="43"/>
+      <c r="C64" s="76" t="s">
+        <v>409</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="E64" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="F64" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="G64" s="43">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="17">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="72"/>
-      <c r="D65" s="46"/>
-      <c r="E65" s="46"/>
-      <c r="F65" s="45"/>
-      <c r="G65" s="47"/>
+      <c r="D65" s="44"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="4"/>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="4"/>
@@ -8142,19 +8218,19 @@
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="72"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="37"/>
-      <c r="G69" s="4"/>
+      <c r="D69" s="46"/>
+      <c r="E69" s="46"/>
+      <c r="F69" s="45"/>
+      <c r="G69" s="47"/>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="72"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="37"/>
-      <c r="G70" s="4"/>
+      <c r="D70" s="46"/>
+      <c r="E70" s="46"/>
+      <c r="F70" s="45"/>
+      <c r="G70" s="47"/>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="4"/>
@@ -9785,70 +9861,89 @@
       <c r="F251" s="37"/>
       <c r="G251" s="4"/>
     </row>
+    <row r="252" spans="1:7">
+      <c r="A252" s="4"/>
+      <c r="B252" s="4"/>
+      <c r="C252" s="72"/>
+      <c r="D252" s="5"/>
+      <c r="E252" s="5"/>
+      <c r="F252" s="37"/>
+      <c r="G252" s="4"/>
+    </row>
+    <row r="253" spans="1:7">
+      <c r="A253" s="4"/>
+      <c r="B253" s="4"/>
+      <c r="C253" s="72"/>
+      <c r="D253" s="5"/>
+      <c r="E253" s="5"/>
+      <c r="F253" s="37"/>
+      <c r="G253" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E59" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E17" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="E56" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="E43" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="E8" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="E20" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="E22" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="E23" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="E12" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="E51" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="E25" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="E27" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="E47" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="E42" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="E13" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="E57" r:id="rId16" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="E54" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="E15" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="E60" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="E48" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="E24" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="E37" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="E41" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="E18" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="E34" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="E5" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="E40" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="E11" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="E6" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="E4" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="E61" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="E58" r:id="rId32" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="E53" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="E31" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="E49" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="E2" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="E14" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="E50" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="E21" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="E28" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="E9" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="E39" r:id="rId42" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="E30" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="E16" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="E3" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="E45" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="E10" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="E52" r:id="rId48" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="E7" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="E46" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="E38" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="E44" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="E19" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
-    <hyperlink ref="E55" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
-    <hyperlink ref="E32" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
-    <hyperlink ref="E36" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
-    <hyperlink ref="E33" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
-    <hyperlink ref="E35" r:id="rId58" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
-    <hyperlink ref="E29" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
-    <hyperlink ref="E62" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
-    <hyperlink ref="E26" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="E61" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E18" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E58" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E45" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E21" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E23" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E24" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E13" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="E53" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="E26" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="E28" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="E49" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="E44" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="E14" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="E59" r:id="rId15" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="E56" r:id="rId16" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="E16" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="E62" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="E50" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="E25" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="E39" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="E43" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="E19" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="E36" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="E5" r:id="rId25" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="E42" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="E12" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="E6" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="E4" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="E63" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="E60" r:id="rId31" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="E55" r:id="rId32" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="E32" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="E51" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="E2" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="E15" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="E52" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="E22" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="E29" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="E10" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="E41" r:id="rId41" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="E31" r:id="rId42" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="E17" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="E3" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="E47" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="E11" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="E54" r:id="rId47" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="E7" r:id="rId48" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="E48" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="E40" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="E46" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="E20" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="E57" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="E33" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="E38" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="E37" r:id="rId56" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="E30" r:id="rId57" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="E64" r:id="rId58" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="E27" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="E34" r:id="rId60" xr:uid="{7EC1841A-D2E4-4D40-85F8-574AF7C9ED0F}"/>
+    <hyperlink ref="E8" r:id="rId61" xr:uid="{5F14C7A6-B6D6-9542-8B33-155349E77E8F}"/>
+    <hyperlink ref="E9" r:id="rId62" xr:uid="{AF98066F-1603-B94A-BA89-552597EAD77F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9875,32 +9970,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="90" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="90" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="84" t="s">
+      <c r="C1" s="90" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="90" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="84" t="s">
+      <c r="E1" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="84" t="s">
+      <c r="F1" s="90" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19" customHeight="1">
-      <c r="A2" s="84"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
+      <c r="A2" s="90"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
     </row>
     <row r="3" spans="1:6" ht="14">
       <c r="A3" s="37">

</xml_diff>